<commit_message>
update cdfw zooplankton filenames
</commit_message>
<xml_diff>
--- a/strends-report/examples/columns.xlsx
+++ b/strends-report/examples/columns.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="422">
   <si>
     <t>flow_index</t>
   </si>
@@ -398,6 +398,9 @@
     <t>DWRStation</t>
   </si>
   <si>
+    <t>DWRStationNo</t>
+  </si>
+  <si>
     <t>WeatherCode</t>
   </si>
   <si>
@@ -479,6 +482,9 @@
     <t>Green Algae</t>
   </si>
   <si>
+    <t>TideCode</t>
+  </si>
+  <si>
     <t>Count</t>
   </si>
   <si>
@@ -557,9 +563,6 @@
     <t>CBMeterStart</t>
   </si>
   <si>
-    <t>TideCode</t>
-  </si>
-  <si>
     <t>Raphidophytes</t>
   </si>
   <si>
@@ -578,219 +581,219 @@
     <t>Red Algae</t>
   </si>
   <si>
+    <t>MysidVolume</t>
+  </si>
+  <si>
+    <t>PumpVolume</t>
+  </si>
+  <si>
+    <t>TowDuration</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>CBMeterCheck</t>
+  </si>
+  <si>
+    <t>MeterNumber</t>
+  </si>
+  <si>
+    <t>Silico-flagellates</t>
+  </si>
+  <si>
+    <t>A_ aspera</t>
+  </si>
+  <si>
+    <t>LIMNOSINE</t>
+  </si>
+  <si>
+    <t>flowDebris</t>
+  </si>
+  <si>
+    <t>TowVolume</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Synurophytes</t>
+  </si>
+  <si>
     <t>CBVolume</t>
   </si>
   <si>
-    <t>MysidVolume</t>
-  </si>
-  <si>
-    <t>PumpVolume</t>
-  </si>
-  <si>
-    <t>TowDuration</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>CBMeterCheck</t>
-  </si>
-  <si>
-    <t>MeterNumber</t>
-  </si>
-  <si>
-    <t>Silico-flagellates</t>
+    <t>A_ hwanhaiensis</t>
+  </si>
+  <si>
+    <t>LIMNOSPP</t>
+  </si>
+  <si>
+    <t>SiteDisturbance</t>
+  </si>
+  <si>
+    <t>AMESHAAge0</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Unknown Algae</t>
   </si>
   <si>
     <t>ACARTELA</t>
   </si>
   <si>
-    <t>A_ aspera</t>
-  </si>
-  <si>
-    <t>LIMNOSINE</t>
-  </si>
-  <si>
-    <t>flowDebris</t>
-  </si>
-  <si>
-    <t>TowVolume</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Synurophytes</t>
+    <t>A_ macropsis</t>
+  </si>
+  <si>
+    <t>LIMNOTET</t>
+  </si>
+  <si>
+    <t>AlternateSite</t>
+  </si>
+  <si>
+    <t>AMESHAAge1+</t>
+  </si>
+  <si>
+    <t>SampleComments</t>
+  </si>
+  <si>
+    <t>Unknown Flagellates</t>
   </si>
   <si>
     <t>ACARTIA</t>
   </si>
   <si>
-    <t>A_ hwanhaiensis</t>
-  </si>
-  <si>
-    <t>LIMNOSPP</t>
-  </si>
-  <si>
-    <t>SiteDisturbance</t>
-  </si>
-  <si>
-    <t>AMESHAAge0</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Unknown Algae</t>
+    <t>D_ holmquistae</t>
+  </si>
+  <si>
+    <t>TotalLimno</t>
+  </si>
+  <si>
+    <t>SeineLength</t>
+  </si>
+  <si>
+    <t>SpCnd</t>
+  </si>
+  <si>
+    <t>AMESHA</t>
+  </si>
+  <si>
+    <t>Xanthophytes</t>
   </si>
   <si>
     <t>DIAPTOM</t>
   </si>
   <si>
-    <t>A_ macropsis</t>
-  </si>
-  <si>
-    <t>LIMNOTET</t>
-  </si>
-  <si>
-    <t>AlternateSite</t>
-  </si>
-  <si>
-    <t>AMESHAAge1+</t>
-  </si>
-  <si>
-    <t>SampleComments</t>
-  </si>
-  <si>
-    <t>Unknown Flagellates</t>
+    <t>H_ longirostris</t>
+  </si>
+  <si>
+    <t>OITHDAV</t>
+  </si>
+  <si>
+    <t>SeineWidth</t>
+  </si>
+  <si>
+    <t>ARRGOB</t>
   </si>
   <si>
     <t>EURYTEM</t>
   </si>
   <si>
-    <t>D_ holmquistae</t>
-  </si>
-  <si>
-    <t>TotalLimno</t>
-  </si>
-  <si>
-    <t>SeineLength</t>
-  </si>
-  <si>
-    <t>SpCnd</t>
-  </si>
-  <si>
-    <t>AMESHA</t>
-  </si>
-  <si>
-    <t>Xanthophytes</t>
+    <t>N_ kadiakensis</t>
+  </si>
+  <si>
+    <t>OITHSIM</t>
+  </si>
+  <si>
+    <t>SeineDepth</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>BARSUR</t>
   </si>
   <si>
     <t>OTHCALAD</t>
   </si>
   <si>
-    <t>H_ longirostris</t>
-  </si>
-  <si>
-    <t>OITHDAV</t>
-  </si>
-  <si>
-    <t>SeineWidth</t>
-  </si>
-  <si>
-    <t>ARRGOB</t>
+    <t>N_ mercedis</t>
+  </si>
+  <si>
+    <t>OITHSPP</t>
+  </si>
+  <si>
+    <t>StartMeter</t>
+  </si>
+  <si>
+    <t>BATRAY</t>
   </si>
   <si>
     <t>PDIAPFOR</t>
   </si>
   <si>
-    <t>N_ kadiakensis</t>
-  </si>
-  <si>
-    <t>OITHSIM</t>
-  </si>
-  <si>
-    <t>SeineDepth</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>BARSUR</t>
+    <t>Unidentified mysid</t>
+  </si>
+  <si>
+    <t>OTHCYCAD</t>
+  </si>
+  <si>
+    <t>EndMeter</t>
+  </si>
+  <si>
+    <t>SubstrateCode</t>
+  </si>
+  <si>
+    <t>BAYGOB</t>
   </si>
   <si>
     <t>PDIAPMAR</t>
   </si>
   <si>
-    <t>N_ mercedis</t>
-  </si>
-  <si>
-    <t>OITHSPP</t>
-  </si>
-  <si>
-    <t>StartMeter</t>
-  </si>
-  <si>
-    <t>BATRAY</t>
+    <t>ALLCYCADULTS</t>
+  </si>
+  <si>
+    <t>TotalMeter</t>
+  </si>
+  <si>
+    <t>BAYPIP</t>
   </si>
   <si>
     <t>SINOCAL</t>
   </si>
   <si>
-    <t>Unidentified mysid</t>
-  </si>
-  <si>
-    <t>OTHCYCAD</t>
-  </si>
-  <si>
-    <t>EndMeter</t>
-  </si>
-  <si>
-    <t>SubstrateCode</t>
-  </si>
-  <si>
-    <t>BAYGOB</t>
+    <t>HARPACT</t>
+  </si>
+  <si>
+    <t>VolumeSeined</t>
+  </si>
+  <si>
+    <t>BIGSKA</t>
   </si>
   <si>
     <t>TORTANUS</t>
   </si>
   <si>
-    <t>ALLCYCADULTS</t>
-  </si>
-  <si>
-    <t>TotalMeter</t>
-  </si>
-  <si>
-    <t>BAYPIP</t>
+    <t>CYCJUV</t>
+  </si>
+  <si>
+    <t>BLABUL</t>
   </si>
   <si>
     <t>ALLCALADULTS</t>
   </si>
   <si>
-    <t>HARPACT</t>
-  </si>
-  <si>
-    <t>VolumeSeined</t>
-  </si>
-  <si>
-    <t>BIGSKA</t>
+    <t>LIMNOJUV</t>
+  </si>
+  <si>
+    <t>BLACRA</t>
   </si>
   <si>
     <t>AVERNAL</t>
   </si>
   <si>
-    <t>CYCJUV</t>
-  </si>
-  <si>
-    <t>BLABUL</t>
-  </si>
-  <si>
-    <t>LIMNOJUV</t>
-  </si>
-  <si>
-    <t>BLACRA</t>
-  </si>
-  <si>
     <t>OITHJUV</t>
   </si>
   <si>
@@ -848,99 +851,99 @@
     <t>BROSSH</t>
   </si>
   <si>
+    <t>ALLCOPNAUP</t>
+  </si>
+  <si>
+    <t>CALGRU</t>
+  </si>
+  <si>
+    <t>ASPLANCH</t>
+  </si>
+  <si>
+    <t>CALHAL</t>
+  </si>
+  <si>
     <t>CALJUV</t>
   </si>
   <si>
-    <t>ALLCOPNAUP</t>
-  </si>
-  <si>
-    <t>CALGRU</t>
+    <t>KERATELA</t>
+  </si>
+  <si>
+    <t>CALLIZ</t>
   </si>
   <si>
     <t>EURYJUV</t>
   </si>
   <si>
-    <t>ASPLANCH</t>
-  </si>
-  <si>
-    <t>CALHAL</t>
+    <t>OTHROT</t>
+  </si>
+  <si>
+    <t>CALSUR</t>
   </si>
   <si>
     <t>OTHCALJUV</t>
   </si>
   <si>
-    <t>KERATELA</t>
-  </si>
-  <si>
-    <t>CALLIZ</t>
+    <t>POLYARTH</t>
+  </si>
+  <si>
+    <t>CALTON</t>
   </si>
   <si>
     <t>PDIAPJUV</t>
   </si>
   <si>
-    <t>OTHROT</t>
-  </si>
-  <si>
-    <t>CALSUR</t>
+    <t>SYNCH</t>
+  </si>
+  <si>
+    <t>CHACAT</t>
   </si>
   <si>
     <t>SINOCALJUV</t>
   </si>
   <si>
-    <t>POLYARTH</t>
-  </si>
-  <si>
-    <t>CALTON</t>
+    <t>SYNCHBIC</t>
+  </si>
+  <si>
+    <t>CHAGOB</t>
   </si>
   <si>
     <t>ASINEJUV</t>
   </si>
   <si>
-    <t>SYNCH</t>
-  </si>
-  <si>
-    <t>CHACAT</t>
+    <t>TRICHO</t>
+  </si>
+  <si>
+    <t>CHEGOB</t>
   </si>
   <si>
     <t>ACARJUV</t>
   </si>
   <si>
-    <t>SYNCHBIC</t>
-  </si>
-  <si>
-    <t>CHAGOB</t>
+    <t>ALLROTIFERS</t>
+  </si>
+  <si>
+    <t>CHISAL</t>
   </si>
   <si>
     <t>DIAPTJUV</t>
   </si>
   <si>
-    <t>TRICHO</t>
-  </si>
-  <si>
-    <t>CHEGOB</t>
+    <t>BARNNAUP</t>
+  </si>
+  <si>
+    <t>COHSAL</t>
   </si>
   <si>
     <t>TORTJUV</t>
   </si>
   <si>
-    <t>ALLROTIFERS</t>
-  </si>
-  <si>
-    <t>CHISAL</t>
+    <t>COMCAR</t>
   </si>
   <si>
     <t>ALLCALJUV</t>
   </si>
   <si>
-    <t>BARNNAUP</t>
-  </si>
-  <si>
-    <t>COHSAL</t>
-  </si>
-  <si>
-    <t>COMCAR</t>
-  </si>
-  <si>
     <t>DELSMEAge0</t>
   </si>
   <si>
@@ -971,39 +974,39 @@
     <t>FLASPP</t>
   </si>
   <si>
+    <t>GOLDFI</t>
+  </si>
+  <si>
+    <t>GOLSHI</t>
+  </si>
+  <si>
     <t>BOSMINA</t>
   </si>
   <si>
-    <t>GOLDFI</t>
+    <t>GRESTU</t>
   </si>
   <si>
     <t>DAPHNIA</t>
   </si>
   <si>
-    <t>GOLSHI</t>
+    <t>GRESUN</t>
   </si>
   <si>
     <t>DIAPHAN</t>
   </si>
   <si>
-    <t>GRESTU</t>
+    <t>HARDHE</t>
   </si>
   <si>
     <t>OTHCLADO</t>
   </si>
   <si>
-    <t>GRESUN</t>
+    <t>HITCH</t>
   </si>
   <si>
     <t>ALLCLADOCERA</t>
   </si>
   <si>
-    <t>HARDHE</t>
-  </si>
-  <si>
-    <t>HITCH</t>
-  </si>
-  <si>
     <t>HORTUR</t>
   </si>
   <si>
@@ -1028,13 +1031,13 @@
     <t>LEOSHA</t>
   </si>
   <si>
+    <t>LINGCO</t>
+  </si>
+  <si>
+    <t>LONSMEAge0</t>
+  </si>
+  <si>
     <t>CRABZOEA</t>
-  </si>
-  <si>
-    <t>LINGCO</t>
-  </si>
-  <si>
-    <t>LONSMEAge0</t>
   </si>
   <si>
     <t>LONSMEAge1+</t>
@@ -2218,74 +2221,74 @@
         <v>126</v>
       </c>
       <c r="G9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J9" t="s">
         <v>66</v>
       </c>
       <c r="K9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M9" t="s"/>
       <c r="N9" t="s"/>
       <c r="O9" t="s"/>
       <c r="P9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Q9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="R9" t="s"/>
       <c r="S9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="T9" t="s"/>
       <c r="U9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V9" t="s">
         <v>55</v>
       </c>
       <c r="W9" t="s"/>
       <c r="X9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Y9" t="s"/>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s"/>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J10" t="s">
         <v>119</v>
@@ -2298,10 +2301,10 @@
       <c r="N10" t="s"/>
       <c r="O10" t="s"/>
       <c r="P10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="R10" t="s"/>
       <c r="S10" t="s">
@@ -2309,43 +2312,43 @@
       </c>
       <c r="T10" t="s"/>
       <c r="U10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="V10" t="s"/>
       <c r="W10" t="s"/>
       <c r="X10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Y10" t="s"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s"/>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
         <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I11" t="s">
         <v>92</v>
       </c>
       <c r="J11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K11" t="s"/>
       <c r="L11" t="s">
@@ -2355,10 +2358,10 @@
       <c r="N11" t="s"/>
       <c r="O11" t="s"/>
       <c r="P11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R11" t="s"/>
       <c r="S11" t="s">
@@ -2366,28 +2369,28 @@
       </c>
       <c r="T11" t="s"/>
       <c r="U11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="V11" t="s"/>
       <c r="W11" t="s"/>
       <c r="X11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Y11" t="s"/>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s"/>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="F12" t="s">
         <v>119</v>
@@ -2396,13 +2399,13 @@
         <v>119</v>
       </c>
       <c r="H12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I12" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J12" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K12" t="s"/>
       <c r="L12" t="s">
@@ -2412,54 +2415,54 @@
       <c r="N12" t="s"/>
       <c r="O12" t="s"/>
       <c r="P12" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="Q12" t="s">
         <v>55</v>
       </c>
       <c r="R12" t="s"/>
       <c r="S12" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="T12" t="s"/>
       <c r="U12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="V12" t="s"/>
       <c r="W12" t="s"/>
       <c r="X12" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="Y12" t="s"/>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s"/>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
         <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E13" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="F13" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G13" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H13" t="s">
         <v>119</v>
       </c>
       <c r="I13" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="K13" t="s"/>
       <c r="L13" t="s"/>
@@ -2467,7 +2470,7 @@
       <c r="N13" t="s"/>
       <c r="O13" t="s"/>
       <c r="P13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="Q13" t="s"/>
       <c r="R13" t="s"/>
@@ -2477,35 +2480,35 @@
       <c r="V13" t="s"/>
       <c r="W13" t="s"/>
       <c r="X13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="Y13" t="s"/>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s"/>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E14" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H14" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="I14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J14" t="s">
         <v>57</v>
@@ -2516,7 +2519,7 @@
       <c r="N14" t="s"/>
       <c r="O14" t="s"/>
       <c r="P14" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="Q14" t="s"/>
       <c r="R14" t="s"/>
@@ -2526,7 +2529,7 @@
       <c r="V14" t="s"/>
       <c r="W14" t="s"/>
       <c r="X14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="Y14" t="s"/>
     </row>
@@ -2534,25 +2537,25 @@
       <c r="A15" t="s"/>
       <c r="B15" t="s"/>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E15" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H15" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J15" t="s">
         <v>75</v>
@@ -2563,7 +2566,7 @@
       <c r="N15" t="s"/>
       <c r="O15" t="s"/>
       <c r="P15" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="Q15" t="s"/>
       <c r="R15" t="s"/>
@@ -2573,7 +2576,7 @@
       <c r="V15" t="s"/>
       <c r="W15" t="s"/>
       <c r="X15" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="Y15" t="s"/>
     </row>
@@ -2584,19 +2587,19 @@
         <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E16" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I16" t="s">
         <v>112</v>
@@ -2610,7 +2613,7 @@
       <c r="N16" t="s"/>
       <c r="O16" t="s"/>
       <c r="P16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Q16" t="s"/>
       <c r="R16" t="s"/>
@@ -2620,7 +2623,7 @@
       <c r="V16" t="s"/>
       <c r="W16" t="s"/>
       <c r="X16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Y16" t="s"/>
     </row>
@@ -2628,13 +2631,13 @@
       <c r="A17" t="s"/>
       <c r="B17" t="s"/>
       <c r="C17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E17" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F17" t="s">
         <v>188</v>
@@ -2646,7 +2649,7 @@
         <v>190</v>
       </c>
       <c r="I17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J17" t="s">
         <v>191</v>
@@ -2675,28 +2678,28 @@
       <c r="A18" t="s"/>
       <c r="B18" t="s"/>
       <c r="C18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D18" t="s">
         <v>194</v>
       </c>
       <c r="E18" t="s">
+        <v>183</v>
+      </c>
+      <c r="F18" t="s">
         <v>195</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>196</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>197</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
+        <v>145</v>
+      </c>
+      <c r="J18" t="s">
         <v>198</v>
-      </c>
-      <c r="I18" t="s">
-        <v>144</v>
-      </c>
-      <c r="J18" t="s">
-        <v>199</v>
       </c>
       <c r="K18" t="s"/>
       <c r="L18" t="s"/>
@@ -2714,7 +2717,7 @@
       <c r="V18" t="s"/>
       <c r="W18" t="s"/>
       <c r="X18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Y18" t="s"/>
     </row>
@@ -2723,25 +2726,25 @@
       <c r="B19" t="s"/>
       <c r="C19" t="s"/>
       <c r="D19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E19" t="s">
         <v>201</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>202</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>203</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>204</v>
-      </c>
-      <c r="H19" t="s">
-        <v>205</v>
       </c>
       <c r="I19" t="s">
         <v>119</v>
       </c>
       <c r="J19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K19" t="s"/>
       <c r="L19" t="s"/>
@@ -2757,7 +2760,7 @@
       <c r="V19" t="s"/>
       <c r="W19" t="s"/>
       <c r="X19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y19" t="s"/>
     </row>
@@ -2766,25 +2769,25 @@
       <c r="B20" t="s"/>
       <c r="C20" t="s"/>
       <c r="D20" t="s">
+        <v>207</v>
+      </c>
+      <c r="E20" t="s">
         <v>208</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>209</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>210</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>211</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
+        <v>172</v>
+      </c>
+      <c r="J20" t="s">
         <v>212</v>
-      </c>
-      <c r="I20" t="s">
-        <v>170</v>
-      </c>
-      <c r="J20" t="s">
-        <v>213</v>
       </c>
       <c r="K20" t="s"/>
       <c r="L20" t="s"/>
@@ -2800,7 +2803,7 @@
       <c r="V20" t="s"/>
       <c r="W20" t="s"/>
       <c r="X20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y20" t="s"/>
     </row>
@@ -2809,25 +2812,25 @@
       <c r="B21" t="s"/>
       <c r="C21" t="s"/>
       <c r="D21" t="s">
+        <v>214</v>
+      </c>
+      <c r="E21" t="s">
         <v>215</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>216</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>217</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>218</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>219</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>220</v>
-      </c>
-      <c r="J21" t="s">
-        <v>221</v>
       </c>
       <c r="K21" t="s"/>
       <c r="L21" t="s"/>
@@ -2850,25 +2853,25 @@
       <c r="B22" t="s"/>
       <c r="C22" t="s"/>
       <c r="D22" t="s">
+        <v>221</v>
+      </c>
+      <c r="E22" t="s">
         <v>222</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>223</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>224</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>225</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
+        <v>140</v>
+      </c>
+      <c r="J22" t="s">
         <v>226</v>
-      </c>
-      <c r="I22" t="s">
-        <v>139</v>
-      </c>
-      <c r="J22" t="s">
-        <v>227</v>
       </c>
       <c r="K22" t="s"/>
       <c r="L22" t="s"/>
@@ -2892,22 +2895,22 @@
       <c r="C23" t="s"/>
       <c r="D23" t="s"/>
       <c r="E23" t="s">
+        <v>227</v>
+      </c>
+      <c r="F23" t="s">
         <v>228</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>229</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>230</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>231</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>232</v>
-      </c>
-      <c r="J23" t="s">
-        <v>233</v>
       </c>
       <c r="K23" t="s"/>
       <c r="L23" t="s"/>
@@ -2931,22 +2934,22 @@
       <c r="C24" t="s"/>
       <c r="D24" t="s"/>
       <c r="E24" t="s">
+        <v>233</v>
+      </c>
+      <c r="F24" t="s">
         <v>234</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>235</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>236</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
+        <v>133</v>
+      </c>
+      <c r="J24" t="s">
         <v>237</v>
-      </c>
-      <c r="I24" t="s">
-        <v>132</v>
-      </c>
-      <c r="J24" t="s">
-        <v>238</v>
       </c>
       <c r="K24" t="s"/>
       <c r="L24" t="s"/>
@@ -2970,22 +2973,22 @@
       <c r="C25" t="s"/>
       <c r="D25" t="s"/>
       <c r="E25" t="s">
+        <v>238</v>
+      </c>
+      <c r="F25" t="s">
         <v>239</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>240</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>241</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>242</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>243</v>
-      </c>
-      <c r="J25" t="s">
-        <v>244</v>
       </c>
       <c r="K25" t="s"/>
       <c r="L25" t="s"/>
@@ -3009,20 +3012,20 @@
       <c r="C26" t="s"/>
       <c r="D26" t="s"/>
       <c r="E26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F26" t="s"/>
       <c r="G26" t="s">
+        <v>245</v>
+      </c>
+      <c r="H26" t="s">
         <v>246</v>
-      </c>
-      <c r="H26" t="s">
-        <v>247</v>
       </c>
       <c r="I26" t="s">
         <v>88</v>
       </c>
       <c r="J26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K26" t="s"/>
       <c r="L26" t="s"/>
@@ -3046,20 +3049,20 @@
       <c r="C27" t="s"/>
       <c r="D27" t="s"/>
       <c r="E27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F27" t="s"/>
       <c r="G27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H27" t="s">
         <v>105</v>
       </c>
       <c r="I27" t="s">
+        <v>250</v>
+      </c>
+      <c r="J27" t="s">
         <v>251</v>
-      </c>
-      <c r="J27" t="s">
-        <v>252</v>
       </c>
       <c r="K27" t="s"/>
       <c r="L27" t="s"/>
@@ -3083,18 +3086,18 @@
       <c r="C28" t="s"/>
       <c r="D28" t="s"/>
       <c r="E28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F28" t="s"/>
       <c r="G28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H28" t="s">
         <v>39</v>
       </c>
       <c r="I28" t="s"/>
       <c r="J28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K28" t="s"/>
       <c r="L28" t="s"/>
@@ -3118,7 +3121,7 @@
       <c r="C29" t="s"/>
       <c r="D29" t="s"/>
       <c r="E29" t="s">
-        <v>204</v>
+        <v>255</v>
       </c>
       <c r="F29" t="s"/>
       <c r="G29" t="s">
@@ -3153,18 +3156,18 @@
       <c r="C30" t="s"/>
       <c r="D30" t="s"/>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>258</v>
       </c>
       <c r="F30" t="s"/>
       <c r="G30" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H30" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I30" t="s"/>
       <c r="J30" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K30" t="s"/>
       <c r="L30" t="s"/>
@@ -3188,18 +3191,18 @@
       <c r="C31" t="s"/>
       <c r="D31" t="s"/>
       <c r="E31" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F31" t="s"/>
       <c r="G31" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I31" t="s"/>
       <c r="J31" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K31" t="s"/>
       <c r="L31" t="s"/>
@@ -3223,18 +3226,18 @@
       <c r="C32" t="s"/>
       <c r="D32" t="s"/>
       <c r="E32" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="F32" t="s"/>
       <c r="G32" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H32" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I32" t="s"/>
       <c r="J32" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K32" t="s"/>
       <c r="L32" t="s"/>
@@ -3258,18 +3261,18 @@
       <c r="C33" t="s"/>
       <c r="D33" t="s"/>
       <c r="E33" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="F33" t="s"/>
       <c r="G33" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H33" t="s">
         <v>92</v>
       </c>
       <c r="I33" t="s"/>
       <c r="J33" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K33" t="s"/>
       <c r="L33" t="s"/>
@@ -3293,18 +3296,18 @@
       <c r="C34" t="s"/>
       <c r="D34" t="s"/>
       <c r="E34" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F34" t="s"/>
       <c r="G34" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H34" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I34" t="s"/>
       <c r="J34" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K34" t="s"/>
       <c r="L34" t="s"/>
@@ -3328,18 +3331,18 @@
       <c r="C35" t="s"/>
       <c r="D35" t="s"/>
       <c r="E35" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F35" t="s"/>
       <c r="G35" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H35" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I35" t="s"/>
       <c r="J35" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="K35" t="s"/>
       <c r="L35" t="s"/>
@@ -3363,16 +3366,16 @@
       <c r="C36" t="s"/>
       <c r="D36" t="s"/>
       <c r="E36" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="F36" t="s"/>
       <c r="G36" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H36" t="s"/>
       <c r="I36" t="s"/>
       <c r="J36" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K36" t="s"/>
       <c r="L36" t="s"/>
@@ -3396,16 +3399,16 @@
       <c r="C37" t="s"/>
       <c r="D37" t="s"/>
       <c r="E37" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F37" t="s"/>
       <c r="G37" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H37" t="s"/>
       <c r="I37" t="s"/>
       <c r="J37" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K37" t="s"/>
       <c r="L37" t="s"/>
@@ -3429,7 +3432,7 @@
       <c r="C38" t="s"/>
       <c r="D38" t="s"/>
       <c r="E38" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="F38" t="s"/>
       <c r="G38" t="s">
@@ -3462,16 +3465,16 @@
       <c r="C39" t="s"/>
       <c r="D39" t="s"/>
       <c r="E39" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="F39" t="s"/>
       <c r="G39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H39" t="s"/>
       <c r="I39" t="s"/>
       <c r="J39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K39" t="s"/>
       <c r="L39" t="s"/>
@@ -3495,16 +3498,16 @@
       <c r="C40" t="s"/>
       <c r="D40" t="s"/>
       <c r="E40" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F40" t="s"/>
       <c r="G40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H40" t="s"/>
       <c r="I40" t="s"/>
       <c r="J40" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K40" t="s"/>
       <c r="L40" t="s"/>
@@ -3528,16 +3531,16 @@
       <c r="C41" t="s"/>
       <c r="D41" t="s"/>
       <c r="E41" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F41" t="s"/>
       <c r="G41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H41" t="s"/>
       <c r="I41" t="s"/>
       <c r="J41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K41" t="s"/>
       <c r="L41" t="s"/>
@@ -3561,16 +3564,16 @@
       <c r="C42" t="s"/>
       <c r="D42" t="s"/>
       <c r="E42" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F42" t="s"/>
       <c r="G42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H42" t="s"/>
       <c r="I42" t="s"/>
       <c r="J42" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K42" t="s"/>
       <c r="L42" t="s"/>
@@ -3594,16 +3597,16 @@
       <c r="C43" t="s"/>
       <c r="D43" t="s"/>
       <c r="E43" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F43" t="s"/>
       <c r="G43" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H43" t="s"/>
       <c r="I43" t="s"/>
       <c r="J43" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K43" t="s"/>
       <c r="L43" t="s"/>
@@ -3627,16 +3630,16 @@
       <c r="C44" t="s"/>
       <c r="D44" t="s"/>
       <c r="E44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F44" t="s"/>
       <c r="G44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H44" t="s"/>
       <c r="I44" t="s"/>
       <c r="J44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K44" t="s"/>
       <c r="L44" t="s"/>
@@ -3660,16 +3663,16 @@
       <c r="C45" t="s"/>
       <c r="D45" t="s"/>
       <c r="E45" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F45" t="s"/>
       <c r="G45" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H45" t="s"/>
       <c r="I45" t="s"/>
       <c r="J45" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K45" t="s"/>
       <c r="L45" t="s"/>
@@ -3693,16 +3696,16 @@
       <c r="C46" t="s"/>
       <c r="D46" t="s"/>
       <c r="E46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F46" t="s"/>
       <c r="G46" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H46" t="s"/>
       <c r="I46" t="s"/>
       <c r="J46" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K46" t="s"/>
       <c r="L46" t="s"/>
@@ -3726,16 +3729,16 @@
       <c r="C47" t="s"/>
       <c r="D47" t="s"/>
       <c r="E47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F47" t="s"/>
       <c r="G47" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H47" t="s"/>
       <c r="I47" t="s"/>
       <c r="J47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K47" t="s"/>
       <c r="L47" t="s"/>
@@ -3759,7 +3762,7 @@
       <c r="C48" t="s"/>
       <c r="D48" t="s"/>
       <c r="E48" t="s">
-        <v>254</v>
+        <v>306</v>
       </c>
       <c r="F48" t="s"/>
       <c r="G48" t="s"/>
@@ -3790,14 +3793,14 @@
       <c r="C49" t="s"/>
       <c r="D49" t="s"/>
       <c r="E49" t="s">
-        <v>256</v>
+        <v>308</v>
       </c>
       <c r="F49" t="s"/>
       <c r="G49" t="s"/>
       <c r="H49" t="s"/>
       <c r="I49" t="s"/>
       <c r="J49" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K49" t="s"/>
       <c r="L49" t="s"/>
@@ -3821,14 +3824,14 @@
       <c r="C50" t="s"/>
       <c r="D50" t="s"/>
       <c r="E50" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F50" t="s"/>
       <c r="G50" t="s"/>
       <c r="H50" t="s"/>
       <c r="I50" t="s"/>
       <c r="J50" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K50" t="s"/>
       <c r="L50" t="s"/>
@@ -3852,14 +3855,14 @@
       <c r="C51" t="s"/>
       <c r="D51" t="s"/>
       <c r="E51" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F51" t="s"/>
       <c r="G51" t="s"/>
       <c r="H51" t="s"/>
       <c r="I51" t="s"/>
       <c r="J51" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K51" t="s"/>
       <c r="L51" t="s"/>
@@ -3883,14 +3886,14 @@
       <c r="C52" t="s"/>
       <c r="D52" t="s"/>
       <c r="E52" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F52" t="s"/>
       <c r="G52" t="s"/>
       <c r="H52" t="s"/>
       <c r="I52" t="s"/>
       <c r="J52" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K52" t="s"/>
       <c r="L52" t="s"/>
@@ -3914,14 +3917,14 @@
       <c r="C53" t="s"/>
       <c r="D53" t="s"/>
       <c r="E53" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F53" t="s"/>
       <c r="G53" t="s"/>
       <c r="H53" t="s"/>
       <c r="I53" t="s"/>
       <c r="J53" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K53" t="s"/>
       <c r="L53" t="s"/>
@@ -3945,14 +3948,14 @@
       <c r="C54" t="s"/>
       <c r="D54" t="s"/>
       <c r="E54" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F54" t="s"/>
       <c r="G54" t="s"/>
       <c r="H54" t="s"/>
       <c r="I54" t="s"/>
       <c r="J54" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="K54" t="s"/>
       <c r="L54" t="s"/>
@@ -3976,14 +3979,14 @@
       <c r="C55" t="s"/>
       <c r="D55" t="s"/>
       <c r="E55" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F55" t="s"/>
       <c r="G55" t="s"/>
       <c r="H55" t="s"/>
       <c r="I55" t="s"/>
       <c r="J55" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K55" t="s"/>
       <c r="L55" t="s"/>
@@ -4007,14 +4010,14 @@
       <c r="C56" t="s"/>
       <c r="D56" t="s"/>
       <c r="E56" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F56" t="s"/>
       <c r="G56" t="s"/>
       <c r="H56" t="s"/>
       <c r="I56" t="s"/>
       <c r="J56" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="K56" t="s"/>
       <c r="L56" t="s"/>
@@ -4038,14 +4041,14 @@
       <c r="C57" t="s"/>
       <c r="D57" t="s"/>
       <c r="E57" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F57" t="s"/>
       <c r="G57" t="s"/>
       <c r="H57" t="s"/>
       <c r="I57" t="s"/>
       <c r="J57" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K57" t="s"/>
       <c r="L57" t="s"/>
@@ -4069,14 +4072,14 @@
       <c r="C58" t="s"/>
       <c r="D58" t="s"/>
       <c r="E58" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F58" t="s"/>
       <c r="G58" t="s"/>
       <c r="H58" t="s"/>
       <c r="I58" t="s"/>
       <c r="J58" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="K58" t="s"/>
       <c r="L58" t="s"/>
@@ -4100,7 +4103,7 @@
       <c r="C59" t="s"/>
       <c r="D59" t="s"/>
       <c r="E59" t="s">
-        <v>318</v>
+        <v>276</v>
       </c>
       <c r="F59" t="s"/>
       <c r="G59" t="s"/>
@@ -4131,14 +4134,14 @@
       <c r="C60" t="s"/>
       <c r="D60" t="s"/>
       <c r="E60" t="s">
-        <v>320</v>
+        <v>278</v>
       </c>
       <c r="F60" t="s"/>
       <c r="G60" t="s"/>
       <c r="H60" t="s"/>
       <c r="I60" t="s"/>
       <c r="J60" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K60" t="s"/>
       <c r="L60" t="s"/>
@@ -4162,14 +4165,14 @@
       <c r="C61" t="s"/>
       <c r="D61" t="s"/>
       <c r="E61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F61" t="s"/>
       <c r="G61" t="s"/>
       <c r="H61" t="s"/>
       <c r="I61" t="s"/>
       <c r="J61" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K61" t="s"/>
       <c r="L61" t="s"/>
@@ -4193,14 +4196,14 @@
       <c r="C62" t="s"/>
       <c r="D62" t="s"/>
       <c r="E62" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F62" t="s"/>
       <c r="G62" t="s"/>
       <c r="H62" t="s"/>
       <c r="I62" t="s"/>
       <c r="J62" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K62" t="s"/>
       <c r="L62" t="s"/>
@@ -4224,14 +4227,14 @@
       <c r="C63" t="s"/>
       <c r="D63" t="s"/>
       <c r="E63" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F63" t="s"/>
       <c r="G63" t="s"/>
       <c r="H63" t="s"/>
       <c r="I63" t="s"/>
       <c r="J63" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K63" t="s"/>
       <c r="L63" t="s"/>
@@ -4255,7 +4258,7 @@
       <c r="C64" t="s"/>
       <c r="D64" t="s"/>
       <c r="E64" t="s">
-        <v>281</v>
+        <v>327</v>
       </c>
       <c r="F64" t="s"/>
       <c r="G64" t="s"/>
@@ -4286,14 +4289,14 @@
       <c r="C65" t="s"/>
       <c r="D65" t="s"/>
       <c r="E65" t="s">
-        <v>284</v>
+        <v>329</v>
       </c>
       <c r="F65" t="s"/>
       <c r="G65" t="s"/>
       <c r="H65" t="s"/>
       <c r="I65" t="s"/>
       <c r="J65" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="K65" t="s"/>
       <c r="L65" t="s"/>
@@ -4317,14 +4320,14 @@
       <c r="C66" t="s"/>
       <c r="D66" t="s"/>
       <c r="E66" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F66" t="s"/>
       <c r="G66" t="s"/>
       <c r="H66" t="s"/>
       <c r="I66" t="s"/>
       <c r="J66" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="K66" t="s"/>
       <c r="L66" t="s"/>
@@ -4348,14 +4351,14 @@
       <c r="C67" t="s"/>
       <c r="D67" t="s"/>
       <c r="E67" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F67" t="s"/>
       <c r="G67" t="s"/>
       <c r="H67" t="s"/>
       <c r="I67" t="s"/>
       <c r="J67" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K67" t="s"/>
       <c r="L67" t="s"/>
@@ -4379,14 +4382,14 @@
       <c r="C68" t="s"/>
       <c r="D68" t="s"/>
       <c r="E68" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="F68" t="s"/>
       <c r="G68" t="s"/>
       <c r="H68" t="s"/>
       <c r="I68" t="s"/>
       <c r="J68" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="K68" t="s"/>
       <c r="L68" t="s"/>
@@ -4410,14 +4413,14 @@
       <c r="C69" t="s"/>
       <c r="D69" t="s"/>
       <c r="E69" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="F69" t="s"/>
       <c r="G69" t="s"/>
       <c r="H69" t="s"/>
       <c r="I69" t="s"/>
       <c r="J69" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K69" t="s"/>
       <c r="L69" t="s"/>
@@ -4441,14 +4444,14 @@
       <c r="C70" t="s"/>
       <c r="D70" t="s"/>
       <c r="E70" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="F70" t="s"/>
       <c r="G70" t="s"/>
       <c r="H70" t="s"/>
       <c r="I70" t="s"/>
       <c r="J70" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K70" t="s"/>
       <c r="L70" t="s"/>
@@ -4472,14 +4475,14 @@
       <c r="C71" t="s"/>
       <c r="D71" t="s"/>
       <c r="E71" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="F71" t="s"/>
       <c r="G71" t="s"/>
       <c r="H71" t="s"/>
       <c r="I71" t="s"/>
       <c r="J71" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K71" t="s"/>
       <c r="L71" t="s"/>
@@ -4503,14 +4506,14 @@
       <c r="C72" t="s"/>
       <c r="D72" t="s"/>
       <c r="E72" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="F72" t="s"/>
       <c r="G72" t="s"/>
       <c r="H72" t="s"/>
       <c r="I72" t="s"/>
       <c r="J72" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K72" t="s"/>
       <c r="L72" t="s"/>
@@ -4534,7 +4537,7 @@
       <c r="C73" t="s"/>
       <c r="D73" t="s"/>
       <c r="E73" t="s">
-        <v>337</v>
+        <v>301</v>
       </c>
       <c r="F73" t="s"/>
       <c r="G73" t="s"/>
@@ -4564,7 +4567,9 @@
       <c r="B74" t="s"/>
       <c r="C74" t="s"/>
       <c r="D74" t="s"/>
-      <c r="E74" t="s"/>
+      <c r="E74" t="s">
+        <v>304</v>
+      </c>
       <c r="F74" t="s"/>
       <c r="G74" t="s"/>
       <c r="H74" t="s"/>
@@ -4593,13 +4598,15 @@
       <c r="B75" t="s"/>
       <c r="C75" t="s"/>
       <c r="D75" t="s"/>
-      <c r="E75" t="s"/>
+      <c r="E75" t="s">
+        <v>340</v>
+      </c>
       <c r="F75" t="s"/>
       <c r="G75" t="s"/>
       <c r="H75" t="s"/>
       <c r="I75" t="s"/>
       <c r="J75" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K75" t="s"/>
       <c r="L75" t="s"/>
@@ -4628,7 +4635,7 @@
       <c r="H76" t="s"/>
       <c r="I76" t="s"/>
       <c r="J76" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K76" t="s"/>
       <c r="L76" t="s"/>
@@ -4657,7 +4664,7 @@
       <c r="H77" t="s"/>
       <c r="I77" t="s"/>
       <c r="J77" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K77" t="s"/>
       <c r="L77" t="s"/>
@@ -4686,7 +4693,7 @@
       <c r="H78" t="s"/>
       <c r="I78" t="s"/>
       <c r="J78" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K78" t="s"/>
       <c r="L78" t="s"/>
@@ -4715,7 +4722,7 @@
       <c r="H79" t="s"/>
       <c r="I79" t="s"/>
       <c r="J79" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="K79" t="s"/>
       <c r="L79" t="s"/>
@@ -4744,7 +4751,7 @@
       <c r="H80" t="s"/>
       <c r="I80" t="s"/>
       <c r="J80" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="K80" t="s"/>
       <c r="L80" t="s"/>
@@ -4773,7 +4780,7 @@
       <c r="H81" t="s"/>
       <c r="I81" t="s"/>
       <c r="J81" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K81" t="s"/>
       <c r="L81" t="s"/>
@@ -4802,7 +4809,7 @@
       <c r="H82" t="s"/>
       <c r="I82" t="s"/>
       <c r="J82" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="K82" t="s"/>
       <c r="L82" t="s"/>
@@ -4831,7 +4838,7 @@
       <c r="H83" t="s"/>
       <c r="I83" t="s"/>
       <c r="J83" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="K83" t="s"/>
       <c r="L83" t="s"/>
@@ -4860,7 +4867,7 @@
       <c r="H84" t="s"/>
       <c r="I84" t="s"/>
       <c r="J84" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="K84" t="s"/>
       <c r="L84" t="s"/>
@@ -4889,7 +4896,7 @@
       <c r="H85" t="s"/>
       <c r="I85" t="s"/>
       <c r="J85" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="K85" t="s"/>
       <c r="L85" t="s"/>
@@ -4918,7 +4925,7 @@
       <c r="H86" t="s"/>
       <c r="I86" t="s"/>
       <c r="J86" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="K86" t="s"/>
       <c r="L86" t="s"/>
@@ -4947,7 +4954,7 @@
       <c r="H87" t="s"/>
       <c r="I87" t="s"/>
       <c r="J87" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="K87" t="s"/>
       <c r="L87" t="s"/>
@@ -4976,7 +4983,7 @@
       <c r="H88" t="s"/>
       <c r="I88" t="s"/>
       <c r="J88" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K88" t="s"/>
       <c r="L88" t="s"/>
@@ -5005,7 +5012,7 @@
       <c r="H89" t="s"/>
       <c r="I89" t="s"/>
       <c r="J89" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="K89" t="s"/>
       <c r="L89" t="s"/>
@@ -5034,7 +5041,7 @@
       <c r="H90" t="s"/>
       <c r="I90" t="s"/>
       <c r="J90" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="K90" t="s"/>
       <c r="L90" t="s"/>
@@ -5063,7 +5070,7 @@
       <c r="H91" t="s"/>
       <c r="I91" t="s"/>
       <c r="J91" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="K91" t="s"/>
       <c r="L91" t="s"/>
@@ -5092,7 +5099,7 @@
       <c r="H92" t="s"/>
       <c r="I92" t="s"/>
       <c r="J92" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="K92" t="s"/>
       <c r="L92" t="s"/>
@@ -5121,7 +5128,7 @@
       <c r="H93" t="s"/>
       <c r="I93" t="s"/>
       <c r="J93" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="K93" t="s"/>
       <c r="L93" t="s"/>
@@ -5150,7 +5157,7 @@
       <c r="H94" t="s"/>
       <c r="I94" t="s"/>
       <c r="J94" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="K94" t="s"/>
       <c r="L94" t="s"/>
@@ -5179,7 +5186,7 @@
       <c r="H95" t="s"/>
       <c r="I95" t="s"/>
       <c r="J95" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="K95" t="s"/>
       <c r="L95" t="s"/>
@@ -5208,7 +5215,7 @@
       <c r="H96" t="s"/>
       <c r="I96" t="s"/>
       <c r="J96" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K96" t="s"/>
       <c r="L96" t="s"/>
@@ -5237,7 +5244,7 @@
       <c r="H97" t="s"/>
       <c r="I97" t="s"/>
       <c r="J97" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K97" t="s"/>
       <c r="L97" t="s"/>
@@ -5266,7 +5273,7 @@
       <c r="H98" t="s"/>
       <c r="I98" t="s"/>
       <c r="J98" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="K98" t="s"/>
       <c r="L98" t="s"/>
@@ -5295,7 +5302,7 @@
       <c r="H99" t="s"/>
       <c r="I99" t="s"/>
       <c r="J99" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K99" t="s"/>
       <c r="L99" t="s"/>
@@ -5324,7 +5331,7 @@
       <c r="H100" t="s"/>
       <c r="I100" t="s"/>
       <c r="J100" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K100" t="s"/>
       <c r="L100" t="s"/>
@@ -5353,7 +5360,7 @@
       <c r="H101" t="s"/>
       <c r="I101" t="s"/>
       <c r="J101" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="K101" t="s"/>
       <c r="L101" t="s"/>
@@ -5382,7 +5389,7 @@
       <c r="H102" t="s"/>
       <c r="I102" t="s"/>
       <c r="J102" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="K102" t="s"/>
       <c r="L102" t="s"/>
@@ -5411,7 +5418,7 @@
       <c r="H103" t="s"/>
       <c r="I103" t="s"/>
       <c r="J103" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="K103" t="s"/>
       <c r="L103" t="s"/>
@@ -5440,7 +5447,7 @@
       <c r="H104" t="s"/>
       <c r="I104" t="s"/>
       <c r="J104" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="K104" t="s"/>
       <c r="L104" t="s"/>
@@ -5469,7 +5476,7 @@
       <c r="H105" t="s"/>
       <c r="I105" t="s"/>
       <c r="J105" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K105" t="s"/>
       <c r="L105" t="s"/>
@@ -5498,7 +5505,7 @@
       <c r="H106" t="s"/>
       <c r="I106" t="s"/>
       <c r="J106" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="K106" t="s"/>
       <c r="L106" t="s"/>
@@ -5527,7 +5534,7 @@
       <c r="H107" t="s"/>
       <c r="I107" t="s"/>
       <c r="J107" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="K107" t="s"/>
       <c r="L107" t="s"/>
@@ -5556,7 +5563,7 @@
       <c r="H108" t="s"/>
       <c r="I108" t="s"/>
       <c r="J108" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="K108" t="s"/>
       <c r="L108" t="s"/>
@@ -5585,7 +5592,7 @@
       <c r="H109" t="s"/>
       <c r="I109" t="s"/>
       <c r="J109" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="K109" t="s"/>
       <c r="L109" t="s"/>
@@ -5614,7 +5621,7 @@
       <c r="H110" t="s"/>
       <c r="I110" t="s"/>
       <c r="J110" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="K110" t="s"/>
       <c r="L110" t="s"/>
@@ -5643,7 +5650,7 @@
       <c r="H111" t="s"/>
       <c r="I111" t="s"/>
       <c r="J111" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K111" t="s"/>
       <c r="L111" t="s"/>
@@ -5672,7 +5679,7 @@
       <c r="H112" t="s"/>
       <c r="I112" t="s"/>
       <c r="J112" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="K112" t="s"/>
       <c r="L112" t="s"/>
@@ -5701,7 +5708,7 @@
       <c r="H113" t="s"/>
       <c r="I113" t="s"/>
       <c r="J113" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="K113" t="s"/>
       <c r="L113" t="s"/>
@@ -5730,7 +5737,7 @@
       <c r="H114" t="s"/>
       <c r="I114" t="s"/>
       <c r="J114" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="K114" t="s"/>
       <c r="L114" t="s"/>
@@ -5759,7 +5766,7 @@
       <c r="H115" t="s"/>
       <c r="I115" t="s"/>
       <c r="J115" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="K115" t="s"/>
       <c r="L115" t="s"/>
@@ -5788,7 +5795,7 @@
       <c r="H116" t="s"/>
       <c r="I116" t="s"/>
       <c r="J116" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="K116" t="s"/>
       <c r="L116" t="s"/>
@@ -5817,7 +5824,7 @@
       <c r="H117" t="s"/>
       <c r="I117" t="s"/>
       <c r="J117" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="K117" t="s"/>
       <c r="L117" t="s"/>
@@ -5846,7 +5853,7 @@
       <c r="H118" t="s"/>
       <c r="I118" t="s"/>
       <c r="J118" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K118" t="s"/>
       <c r="L118" t="s"/>
@@ -5875,7 +5882,7 @@
       <c r="H119" t="s"/>
       <c r="I119" t="s"/>
       <c r="J119" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K119" t="s"/>
       <c r="L119" t="s"/>
@@ -5904,7 +5911,7 @@
       <c r="H120" t="s"/>
       <c r="I120" t="s"/>
       <c r="J120" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="K120" t="s"/>
       <c r="L120" t="s"/>
@@ -5933,7 +5940,7 @@
       <c r="H121" t="s"/>
       <c r="I121" t="s"/>
       <c r="J121" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K121" t="s"/>
       <c r="L121" t="s"/>
@@ -5962,7 +5969,7 @@
       <c r="H122" t="s"/>
       <c r="I122" t="s"/>
       <c r="J122" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="K122" t="s"/>
       <c r="L122" t="s"/>
@@ -5991,7 +5998,7 @@
       <c r="H123" t="s"/>
       <c r="I123" t="s"/>
       <c r="J123" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="K123" t="s"/>
       <c r="L123" t="s"/>
@@ -6020,7 +6027,7 @@
       <c r="H124" t="s"/>
       <c r="I124" t="s"/>
       <c r="J124" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="K124" t="s"/>
       <c r="L124" t="s"/>
@@ -6049,7 +6056,7 @@
       <c r="H125" t="s"/>
       <c r="I125" t="s"/>
       <c r="J125" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="K125" t="s"/>
       <c r="L125" t="s"/>
@@ -6078,7 +6085,7 @@
       <c r="H126" t="s"/>
       <c r="I126" t="s"/>
       <c r="J126" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K126" t="s"/>
       <c r="L126" t="s"/>
@@ -6107,7 +6114,7 @@
       <c r="H127" t="s"/>
       <c r="I127" t="s"/>
       <c r="J127" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="K127" t="s"/>
       <c r="L127" t="s"/>
@@ -6136,7 +6143,7 @@
       <c r="H128" t="s"/>
       <c r="I128" t="s"/>
       <c r="J128" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="K128" t="s"/>
       <c r="L128" t="s"/>
@@ -6165,7 +6172,7 @@
       <c r="H129" t="s"/>
       <c r="I129" t="s"/>
       <c r="J129" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="K129" t="s"/>
       <c r="L129" t="s"/>
@@ -6194,7 +6201,7 @@
       <c r="H130" t="s"/>
       <c r="I130" t="s"/>
       <c r="J130" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="K130" t="s"/>
       <c r="L130" t="s"/>
@@ -6223,7 +6230,7 @@
       <c r="H131" t="s"/>
       <c r="I131" t="s"/>
       <c r="J131" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K131" t="s"/>
       <c r="L131" t="s"/>
@@ -6252,7 +6259,7 @@
       <c r="H132" t="s"/>
       <c r="I132" t="s"/>
       <c r="J132" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="K132" t="s"/>
       <c r="L132" t="s"/>
@@ -6281,7 +6288,7 @@
       <c r="H133" t="s"/>
       <c r="I133" t="s"/>
       <c r="J133" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="K133" t="s"/>
       <c r="L133" t="s"/>
@@ -6310,7 +6317,7 @@
       <c r="H134" t="s"/>
       <c r="I134" t="s"/>
       <c r="J134" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="K134" t="s"/>
       <c r="L134" t="s"/>
@@ -6339,7 +6346,7 @@
       <c r="H135" t="s"/>
       <c r="I135" t="s"/>
       <c r="J135" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="K135" t="s"/>
       <c r="L135" t="s"/>
@@ -6368,7 +6375,7 @@
       <c r="H136" t="s"/>
       <c r="I136" t="s"/>
       <c r="J136" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="K136" t="s"/>
       <c r="L136" t="s"/>
@@ -6397,7 +6404,7 @@
       <c r="H137" t="s"/>
       <c r="I137" t="s"/>
       <c r="J137" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="K137" t="s"/>
       <c r="L137" t="s"/>
@@ -6426,7 +6433,7 @@
       <c r="H138" t="s"/>
       <c r="I138" t="s"/>
       <c r="J138" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="K138" t="s"/>
       <c r="L138" t="s"/>
@@ -6455,7 +6462,7 @@
       <c r="H139" t="s"/>
       <c r="I139" t="s"/>
       <c r="J139" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="K139" t="s"/>
       <c r="L139" t="s"/>
@@ -6484,7 +6491,7 @@
       <c r="H140" t="s"/>
       <c r="I140" t="s"/>
       <c r="J140" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="K140" t="s"/>
       <c r="L140" t="s"/>
@@ -6513,7 +6520,7 @@
       <c r="H141" t="s"/>
       <c r="I141" t="s"/>
       <c r="J141" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="K141" t="s"/>
       <c r="L141" t="s"/>
@@ -6542,7 +6549,7 @@
       <c r="H142" t="s"/>
       <c r="I142" t="s"/>
       <c r="J142" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="K142" t="s"/>
       <c r="L142" t="s"/>
@@ -6571,7 +6578,7 @@
       <c r="H143" t="s"/>
       <c r="I143" t="s"/>
       <c r="J143" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K143" t="s"/>
       <c r="L143" t="s"/>
@@ -6600,7 +6607,7 @@
       <c r="H144" t="s"/>
       <c r="I144" t="s"/>
       <c r="J144" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="K144" t="s"/>
       <c r="L144" t="s"/>
@@ -6629,7 +6636,7 @@
       <c r="H145" t="s"/>
       <c r="I145" t="s"/>
       <c r="J145" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="K145" t="s"/>
       <c r="L145" t="s"/>
@@ -6658,7 +6665,7 @@
       <c r="H146" t="s"/>
       <c r="I146" t="s"/>
       <c r="J146" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="K146" t="s"/>
       <c r="L146" t="s"/>
@@ -6687,7 +6694,7 @@
       <c r="H147" t="s"/>
       <c r="I147" t="s"/>
       <c r="J147" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="K147" t="s"/>
       <c r="L147" t="s"/>
@@ -6716,7 +6723,7 @@
       <c r="H148" t="s"/>
       <c r="I148" t="s"/>
       <c r="J148" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="K148" t="s"/>
       <c r="L148" t="s"/>
@@ -6745,7 +6752,7 @@
       <c r="H149" t="s"/>
       <c r="I149" t="s"/>
       <c r="J149" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="K149" t="s"/>
       <c r="L149" t="s"/>
@@ -6774,7 +6781,7 @@
       <c r="H150" t="s"/>
       <c r="I150" t="s"/>
       <c r="J150" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="K150" t="s"/>
       <c r="L150" t="s"/>
@@ -6803,7 +6810,7 @@
       <c r="H151" t="s"/>
       <c r="I151" t="s"/>
       <c r="J151" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="K151" t="s"/>
       <c r="L151" t="s"/>
@@ -6832,7 +6839,7 @@
       <c r="H152" t="s"/>
       <c r="I152" t="s"/>
       <c r="J152" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="K152" t="s"/>
       <c r="L152" t="s"/>
@@ -6861,7 +6868,7 @@
       <c r="H153" t="s"/>
       <c r="I153" t="s"/>
       <c r="J153" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K153" t="s"/>
       <c r="L153" t="s"/>
@@ -6890,7 +6897,7 @@
       <c r="H154" t="s"/>
       <c r="I154" t="s"/>
       <c r="J154" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="K154" t="s"/>
       <c r="L154" t="s"/>
@@ -6919,7 +6926,7 @@
       <c r="H155" t="s"/>
       <c r="I155" t="s"/>
       <c r="J155" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="K155" t="s"/>
       <c r="L155" t="s"/>

</xml_diff>